<commit_message>
Moved Game Manager Descriptor to correct folder
</commit_message>
<xml_diff>
--- a/Project Documents/GameManagerDescription.xlsx
+++ b/Project Documents/GameManagerDescription.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00194492\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00194492\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Describe Role in game</t>
   </si>
@@ -50,12 +50,6 @@
     <t xml:space="preserve">Name of InterFace </t>
   </si>
   <si>
-    <t>Text description of role in game</t>
-  </si>
-  <si>
-    <t>Text Description</t>
-  </si>
-  <si>
     <t>https://unity3d.com/learn/tutorials/topics/scripting/interfaces</t>
   </si>
   <si>
@@ -71,7 +65,31 @@
     <t>Game Manager</t>
   </si>
   <si>
-    <t>Item Name (Michael)</t>
+    <t>Item Name (Michael Edgar)</t>
+  </si>
+  <si>
+    <t>The role of the game manager is to keep track of the current score, high score and lives count</t>
+  </si>
+  <si>
+    <t>Communicate with the Pop up Score to update the current score, the world when the player</t>
+  </si>
+  <si>
+    <t>dies to update the current lives and the update the high score when necessary</t>
+  </si>
+  <si>
+    <t>Screen display of score, high score and lives</t>
+  </si>
+  <si>
+    <t>Receive score update from the pop up score when the player interacts with an item and receive</t>
+  </si>
+  <si>
+    <t>update when player dies</t>
+  </si>
+  <si>
+    <t>Pop up score and player</t>
+  </si>
+  <si>
+    <t>Display/UI</t>
   </si>
 </sst>
 </file>
@@ -389,89 +407,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" customWidth="1"/>
+    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="3" max="3" width="88.5703125" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="41" hidden="1" customWidth="1"/>
+    <col min="8" max="26" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Game Manager File
</commit_message>
<xml_diff>
--- a/Project Documents/GameManagerDescription.xlsx
+++ b/Project Documents/GameManagerDescription.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00194492\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00194492\Desktop\Push-Penguin3D\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,9 +68,6 @@
     <t>Item Name (Michael Edgar)</t>
   </si>
   <si>
-    <t>The role of the game manager is to keep track of the current score, high score and lives count</t>
-  </si>
-  <si>
     <t>Communicate with the Pop up Score to update the current score, the world when the player</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Display/UI</t>
+  </si>
+  <si>
+    <t>The role of the game manager is to keep track of score values, death parmeters, level diffculty etc.</t>
   </si>
 </sst>
 </file>
@@ -410,13 +410,13 @@
   <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" customWidth="1"/>
-    <col min="2" max="2" width="85.42578125" customWidth="1"/>
+    <col min="2" max="2" width="87.85546875" customWidth="1"/>
     <col min="3" max="3" width="88.5703125" customWidth="1"/>
     <col min="4" max="4" width="39.42578125" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" hidden="1" customWidth="1"/>
@@ -437,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -445,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -461,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -497,10 +497,10 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
         <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated file, Version 2
</commit_message>
<xml_diff>
--- a/Project Documents/GameManagerDescription.xlsx
+++ b/Project Documents/GameManagerDescription.xlsx
@@ -68,15 +68,6 @@
     <t>Item Name (Michael Edgar)</t>
   </si>
   <si>
-    <t>Communicate with the Pop up Score to update the current score, the world when the player</t>
-  </si>
-  <si>
-    <t>dies to update the current lives and the update the high score when necessary</t>
-  </si>
-  <si>
-    <t>Screen display of score, high score and lives</t>
-  </si>
-  <si>
     <t>Receive score update from the pop up score when the player interacts with an item and receive</t>
   </si>
   <si>
@@ -89,7 +80,16 @@
     <t>Display/UI</t>
   </si>
   <si>
-    <t>The role of the game manager is to keep track of score values, death parmeters, level diffculty etc.</t>
+    <t>Communicate with the pop up score to tell it what value to display when  the player collides with</t>
+  </si>
+  <si>
+    <t>The role of the game manager is to keep track of score values, death parmeters, level diffculty</t>
+  </si>
+  <si>
+    <t>an item. Communicate with the player when it collides with an enemy to display the death.</t>
+  </si>
+  <si>
+    <t>It also instansiates the game objects and asks the world where to spawn them.</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:Z16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,6 +437,9 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -445,24 +448,21 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -497,10 +497,10 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final Game Manager Description
</commit_message>
<xml_diff>
--- a/Project Documents/GameManagerDescription.xlsx
+++ b/Project Documents/GameManagerDescription.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Describe Role in game</t>
   </si>
@@ -32,21 +32,12 @@
     <t>Internal Functionality</t>
   </si>
   <si>
-    <t>Eg Turn Left</t>
-  </si>
-  <si>
     <t>External Outgoing</t>
   </si>
   <si>
-    <t>Eg Push</t>
-  </si>
-  <si>
     <t>External Incoming</t>
   </si>
   <si>
-    <t>ShouldTurnLeft</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name of InterFace </t>
   </si>
   <si>
@@ -68,38 +59,109 @@
     <t>Item Name (Michael Edgar)</t>
   </si>
   <si>
-    <t>Receive score update from the pop up score when the player interacts with an item and receive</t>
-  </si>
-  <si>
-    <t>update when player dies</t>
-  </si>
-  <si>
-    <t>Pop up score and player</t>
-  </si>
-  <si>
-    <t>Display/UI</t>
-  </si>
-  <si>
-    <t>Communicate with the pop up score to tell it what value to display when  the player collides with</t>
-  </si>
-  <si>
-    <t>The role of the game manager is to keep track of score values, death parmeters, level diffculty</t>
-  </si>
-  <si>
-    <t>an item. Communicate with the player when it collides with an enemy to display the death.</t>
-  </si>
-  <si>
     <t>It also instansiates the game objects and asks the world where to spawn them.</t>
+  </si>
+  <si>
+    <t>Text Description</t>
+  </si>
+  <si>
+    <t>The role of the game manager is to keep track of score values, death parmeters, level diffculty.</t>
+  </si>
+  <si>
+    <t>Spawn Items</t>
+  </si>
+  <si>
+    <t>Spawn the eggs, ice blocks, enemies, rocks, player, score and pickup items at the start of the level</t>
+  </si>
+  <si>
+    <t>Set position</t>
+  </si>
+  <si>
+    <t>Set the position of the items by communicating with the World</t>
+  </si>
+  <si>
+    <t>Value Display</t>
+  </si>
+  <si>
+    <t>Communicate with the pop up score to tell it what value to display when  the player and enemy collide.</t>
+  </si>
+  <si>
+    <t>Player Death</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Communicate with the enemy to increase movement speed/difficulty.</t>
+  </si>
+  <si>
+    <t>Egg spawn</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Pop Up Score</t>
+  </si>
+  <si>
+    <t>Communicate with the player when it collides with an enemy to despawn.</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Enemy Death</t>
+  </si>
+  <si>
+    <t>Communicate with the enemy when it collides with an ice block to tell it to despawn.</t>
+  </si>
+  <si>
+    <t>Communicate with the egg to tell it when to hatch/spawn an enemy.</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Egg Death</t>
+  </si>
+  <si>
+    <t>Communicate with the egg when something collides with it to tell it to despawn.</t>
+  </si>
+  <si>
+    <t>Score update</t>
+  </si>
+  <si>
+    <t>Pop up score</t>
+  </si>
+  <si>
+    <t>Receive score update from the player when the player interacts with an item.</t>
+  </si>
+  <si>
+    <t>Win/Lose Screen</t>
+  </si>
+  <si>
+    <t>Receive update when player dies to display lose screen or when the player meets the win condition</t>
+  </si>
+  <si>
+    <t>to display the win screen.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,13 +184,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -407,18 +473,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" customWidth="1"/>
-    <col min="2" max="2" width="87.85546875" customWidth="1"/>
-    <col min="3" max="3" width="88.5703125" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="91.42578125" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" customWidth="1"/>
+    <col min="4" max="4" width="107.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" hidden="1" customWidth="1"/>
     <col min="6" max="7" width="41" hidden="1" customWidth="1"/>
     <col min="8" max="26" width="9.140625" hidden="1" customWidth="1"/>
@@ -426,10 +492,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -437,81 +503,169 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
         <v>7</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D23" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>